<commit_message>
small cosmetic changes to make the codebase easier to understand and small bugs fixed that do not change the results
</commit_message>
<xml_diff>
--- a/data/raw/grouping/definitions_experience_change.xlsx
+++ b/data/raw/grouping/definitions_experience_change.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,7 +401,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>consult statistician</t>
+          <t>planning with experts, consult statistician</t>
         </is>
       </c>
     </row>
@@ -468,82 +468,70 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>plan</t>
+          <t>provide documentation</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>planning with experts</t>
+          <t>detailed documentation, detailed code documentation</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>provide documentation</t>
+          <t>provide training</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>detailed documentation, detailed code documentation</t>
+          <t>supervise students, hands on management, train team, provide adequate training</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>provide training</t>
+          <t>replicate</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>supervise students, hands on management, train team, provide adequate training</t>
+          <t>replicate your experiments</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>replicate</t>
+          <t>share data</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>replicate your experiments</t>
+          <t>send raw scans to journals</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>share data</t>
+          <t>use stricter protocols</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>send raw scans to journals</t>
+          <t>sticter protocols</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>use stricter protocols</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
-        <is>
-          <t>sticter protocols</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>validate</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
         <is>
           <t>check raw data, check multiple times, ask for independent reviewers, compare against similar published results, be systematic, independent review of raw data, double check code, multiple data validity checks, check accuracy, checking against published results, review data, validate compound data by group members, corresponding author checking the whole project, use independent validators for quality control, check statistics by team members and experts</t>
         </is>

</xml_diff>